<commit_message>
Added temp values for testing
</commit_message>
<xml_diff>
--- a/Tom/AF_Register_Bank_Member.xlsx
+++ b/Tom/AF_Register_Bank_Member.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ScrumbagsRepos\AF-Testing\Tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1440AFB5-AF23-47B7-B55A-D1A55BE5361F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB20923-29B2-4BB8-B8FA-7EFF184DEC77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TH_TC001" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterBank" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="91">
   <si>
     <t>DT_firstname</t>
   </si>
@@ -107,12 +107,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>1231231234</t>
-  </si>
-  <si>
-    <t>H123124</t>
-  </si>
-  <si>
     <t>123123</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>12532</t>
   </si>
   <si>
-    <t>H123125</t>
-  </si>
-  <si>
     <t>124 West Street</t>
   </si>
   <si>
@@ -159,6 +150,165 @@
   </si>
   <si>
     <t>thomas.a.hennessey@outlook.com</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TH_TC001</t>
+  </si>
+  <si>
+    <t>TH_TC002</t>
+  </si>
+  <si>
+    <t>TH_TC003</t>
+  </si>
+  <si>
+    <t>TH_TC004</t>
+  </si>
+  <si>
+    <t>TH_TC005</t>
+  </si>
+  <si>
+    <t>TH_TC006</t>
+  </si>
+  <si>
+    <t>TH_TC007</t>
+  </si>
+  <si>
+    <t>TH_TC008</t>
+  </si>
+  <si>
+    <t>TH_TC009</t>
+  </si>
+  <si>
+    <t>TH_TC010</t>
+  </si>
+  <si>
+    <t>TH_TC011</t>
+  </si>
+  <si>
+    <t>TH_TC012</t>
+  </si>
+  <si>
+    <t>TH_TC013</t>
+  </si>
+  <si>
+    <t>TH_TC014</t>
+  </si>
+  <si>
+    <t>TH_TC015</t>
+  </si>
+  <si>
+    <t>TH_TC001_R</t>
+  </si>
+  <si>
+    <t>TH_TC002_R</t>
+  </si>
+  <si>
+    <t>TH_TC003_R</t>
+  </si>
+  <si>
+    <t>TH_TC004_R</t>
+  </si>
+  <si>
+    <t>TH_TC005_R</t>
+  </si>
+  <si>
+    <t>TH_TC006_R</t>
+  </si>
+  <si>
+    <t>TH_TC007_R</t>
+  </si>
+  <si>
+    <t>TH_TC008_R</t>
+  </si>
+  <si>
+    <t>TH_TC010_R</t>
+  </si>
+  <si>
+    <t>TH_TC011_R</t>
+  </si>
+  <si>
+    <t>TH_TC009_R</t>
+  </si>
+  <si>
+    <t>TH_TC012_R</t>
+  </si>
+  <si>
+    <t>TH_TC013_R</t>
+  </si>
+  <si>
+    <t>TH_TC014_R</t>
+  </si>
+  <si>
+    <t>TH_TC015_R</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom </t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>STASHING</t>
+  </si>
+  <si>
+    <t>01012200</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>&lt;&lt;</t>
+  </si>
+  <si>
+    <t>125 West Street</t>
+  </si>
+  <si>
+    <t>126 West Street</t>
+  </si>
+  <si>
+    <t>127 West Street</t>
+  </si>
+  <si>
+    <t>128 West Street</t>
+  </si>
+  <si>
+    <t>129 West Street</t>
+  </si>
+  <si>
+    <t>130 West Street</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>123124</t>
+  </si>
+  <si>
+    <t>123125</t>
+  </si>
+  <si>
+    <t>123126</t>
+  </si>
+  <si>
+    <t>123127</t>
+  </si>
+  <si>
+    <t>123128</t>
+  </si>
+  <si>
+    <t>123129</t>
+  </si>
+  <si>
+    <t>123130</t>
   </si>
 </sst>
 </file>
@@ -209,13 +359,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,222 +647,1156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" style="5" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="Q1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>6952258375</v>
+      </c>
+      <c r="I2" s="5">
+        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
+        <v>672894984</v>
+      </c>
+      <c r="J2" s="5">
+        <f ca="1">RANDBETWEEN(1000000,99999999)</f>
+        <v>14886076</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>5148225655</v>
+      </c>
+      <c r="I3" s="5">
+        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
+        <v>957068657</v>
+      </c>
+      <c r="J3" s="5">
+        <f ca="1">RANDBETWEEN(1000000,99999999)</f>
+        <v>24875944</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>2646981136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H13" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>8542726901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>3159189923</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>3529349610</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>8683281250</v>
+      </c>
+      <c r="I18" s="5">
+        <v>123</v>
+      </c>
+      <c r="J18" s="5">
+        <f ca="1">RANDBETWEEN(1000000,99999999)</f>
+        <v>25227225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>9738120704</v>
+      </c>
+      <c r="I19" s="5">
+        <v>123</v>
+      </c>
+      <c r="J19" s="5">
+        <f ca="1">RANDBETWEEN(1000000,99999999)</f>
+        <v>80085895</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>5211948342</v>
+      </c>
+      <c r="I20" s="5">
+        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
+        <v>747273194</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>8527797792</v>
+      </c>
+      <c r="I21" s="5">
+        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
+        <v>554358199</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="5">
+        <f ca="1">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>9720954507</v>
+      </c>
+      <c r="I22" s="5">
+        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
+        <v>254611812</v>
+      </c>
+      <c r="J22" s="5">
+        <f ca="1">RANDBETWEEN(1000000,99999999)</f>
+        <v>91110990</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ref="H23:H31" ca="1" si="0">RANDBETWEEN(1111111111,9999999999)</f>
+        <v>1645189041</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" ref="I23:I31" ca="1" si="1">RANDBETWEEN(111111111,999999999)</f>
+        <v>623456622</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" ref="J23:J31" ca="1" si="2">RANDBETWEEN(1000000,99999999)</f>
+        <v>3530862</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2894474736</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>297332062</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>28487596</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5">
-        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
-        <v>949418402</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="M24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1" t="s">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9259212285</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>680563421</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>2907184</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8633496944</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>341036850</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>33781106</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="5">
-        <f ca="1">RANDBETWEEN(111111111,999999999)</f>
-        <v>416245694</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="P26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9518318161</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>342485227</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>53810973</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5962348701</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>348247711</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>58769740</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="O28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>9601727795</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>779307014</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>73821933</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5601148858</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>590234546</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>62449986</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>34</v>
+      <c r="P30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3289431295</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" ca="1" si="1"/>
+        <v>550808894</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>34925471</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>